<commit_message>
Atualização do Plano GQA
</commit_message>
<xml_diff>
--- a/02-Projeto/01-ResolveAi/02-GQA/02-PlanoGQA.xlsx
+++ b/02-Projeto/01-ResolveAi/02-GQA/02-PlanoGQA.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="555" windowWidth="19815" windowHeight="7365"/>
+    <workbookView xWindow="390" yWindow="555" windowWidth="19815" windowHeight="7365" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tarefas" sheetId="2" r:id="rId1"/>
@@ -95,9 +95,6 @@
     <t>Planejar a correção das não-conformidades</t>
   </si>
   <si>
-    <t>Plano de correção das não conformidades</t>
-  </si>
-  <si>
     <t>Realizar as correções necessárias</t>
   </si>
   <si>
@@ -105,6 +102,9 @@
   </si>
   <si>
     <t>Comunicar os interessados</t>
+  </si>
+  <si>
+    <t>Plano de correção das não-conformidades</t>
   </si>
 </sst>
 </file>
@@ -616,8 +616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D1:D1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -695,7 +695,7 @@
         <v>24</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -706,7 +706,7 @@
         <v>17</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>16</v>
@@ -720,7 +720,7 @@
         <v>18</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D8" s="13" t="s">
         <v>16</v>
@@ -730,7 +730,7 @@
       <c r="A9" s="12"/>
       <c r="B9" s="12"/>
       <c r="C9" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D9" s="18"/>
     </row>
@@ -751,8 +751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>